<commit_message>
ok interp works but only for constants
</commit_message>
<xml_diff>
--- a/tests/databooks/databook_sir.xlsx
+++ b/tests/databooks/databook_sir.xlsx
@@ -1194,8 +1194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1351,18 +1351,12 @@
         <f>'Population Definitions'!B2</f>
         <v>Adults</v>
       </c>
-      <c r="B5" t="str">
+      <c r="B5">
         <f>IF(SUMPRODUCT(--(D5:V5&lt;&gt;""))=0,0.008,"N.A.")</f>
-        <v>N.A.</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="S5">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="T5">
-        <v>8.9999999999999993E-3</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Extracting data into parameters
Continuing to mash TB model run operations with current codebase. This commit deals with assumption issues.
After this, porting interpolateFunc is next.
Note: Framework and test file updates have been applied, aiming to get the SIR model operational.
</commit_message>
<xml_diff>
--- a/tests/databooks/databook_sir.xlsx
+++ b/tests/databooks/databook_sir.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28615"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robynstuart/Documents/git/atomica/tests/databooks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects - Work\Optima\atomica\tests\databooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15842171-212B-49DD-A00B-809DFB4AC454}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="458" windowWidth="16103" windowHeight="9660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Population Definitions" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
     <sheet name="State Variables" sheetId="3" r:id="rId3"/>
     <sheet name="Parameters" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -30,12 +31,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -50,7 +51,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -70,12 +71,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -90,7 +91,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -110,12 +111,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{4E28D499-99B0-415D-A844-70DF33B1D3F8}">
       <text>
         <r>
           <rPr>
@@ -128,7 +129,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{4BA341A9-7098-45BF-BBCF-86B0B36F0886}">
       <text>
         <r>
           <rPr>
@@ -145,7 +146,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A3" authorId="0">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -158,7 +159,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0">
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -175,7 +176,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0">
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -188,7 +189,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="0">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
       <text>
         <r>
           <rPr>
@@ -205,7 +206,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0">
+    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
       <text>
         <r>
           <rPr>
@@ -218,7 +219,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0">
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000006000000}">
       <text>
         <r>
           <rPr>
@@ -235,7 +236,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A9" authorId="0">
+    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000007000000}">
       <text>
         <r>
           <rPr>
@@ -248,7 +249,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0">
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000008000000}">
       <text>
         <r>
           <rPr>
@@ -265,7 +266,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A11" authorId="0">
+    <comment ref="A13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000009000000}">
       <text>
         <r>
           <rPr>
@@ -278,7 +279,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="0">
+    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -295,17 +296,47 @@
         </r>
       </text>
     </comment>
+    <comment ref="A15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000B000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is a characteristic.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000C000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column should be filled with default values used by the model.
+If the option to provide time-dependent values exists, then this can be considered a time-independent assumption.
+In this case, if any time-dependent values are entered, the Excel sheet will attempt to explicitly mark the corresponding cell as inapplicable.
+Alternatively, the user can leave the cell blank.
+However, any other value will override the time-dependent values during a model run.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -318,7 +349,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -335,7 +366,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
       <text>
         <r>
           <rPr>
@@ -348,7 +379,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0">
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
       <text>
         <r>
           <rPr>
@@ -365,7 +396,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0">
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000005000000}">
       <text>
         <r>
           <rPr>
@@ -378,7 +409,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000006000000}">
       <text>
         <r>
           <rPr>
@@ -395,7 +426,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A10" authorId="0">
+    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000007000000}">
       <text>
         <r>
           <rPr>
@@ -408,7 +439,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="0">
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000008000000}">
       <text>
         <r>
           <rPr>
@@ -425,7 +456,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A13" authorId="0">
+    <comment ref="A13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000009000000}">
       <text>
         <r>
           <rPr>
@@ -438,7 +469,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B13" authorId="0">
+    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -455,7 +486,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A16" authorId="0">
+    <comment ref="A16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -468,7 +499,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B16" authorId="0">
+    <comment ref="B16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -485,7 +516,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A19" authorId="0">
+    <comment ref="A19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -498,7 +529,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B19" authorId="0">
+    <comment ref="B19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -520,7 +551,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
   <si>
     <t>Abbreviation</t>
   </si>
@@ -595,12 +626,18 @@
   </si>
   <si>
     <t>Number not at risk of infection</t>
+  </si>
+  <si>
+    <t>Total number of entities</t>
+  </si>
+  <si>
+    <t>N.A.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -661,6 +698,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -952,19 +992,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="2" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -972,7 +1012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
@@ -987,17 +1027,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="2" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1005,7 +1045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1013,7 +1053,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1021,7 +1061,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1036,22 +1076,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:V15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="50.6640625" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>8</v>
@@ -1114,139 +1154,104 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="str">
+        <f>'Population Definitions'!B$2</f>
+        <v>Adults</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2000</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2001</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2002</v>
+      </c>
+      <c r="G4" s="1">
+        <v>2003</v>
+      </c>
+      <c r="H4" s="1">
+        <v>2004</v>
+      </c>
+      <c r="I4" s="1">
+        <v>2005</v>
+      </c>
+      <c r="J4" s="1">
+        <v>2006</v>
+      </c>
+      <c r="K4" s="1">
+        <v>2007</v>
+      </c>
+      <c r="L4" s="1">
+        <v>2008</v>
+      </c>
+      <c r="M4" s="1">
+        <v>2009</v>
+      </c>
+      <c r="N4" s="1">
+        <v>2010</v>
+      </c>
+      <c r="O4" s="1">
+        <v>2011</v>
+      </c>
+      <c r="P4" s="1">
+        <v>2012</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>2013</v>
+      </c>
+      <c r="R4" s="1">
+        <v>2014</v>
+      </c>
+      <c r="S4" s="1">
+        <v>2015</v>
+      </c>
+      <c r="T4" s="1">
+        <v>2016</v>
+      </c>
+      <c r="U4" s="1">
+        <v>2017</v>
+      </c>
+      <c r="V4" s="1">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="str">
+        <f>'Population Definitions'!B$2</f>
+        <v>Adults</v>
+      </c>
+      <c r="B5">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1">
-        <v>2000</v>
-      </c>
-      <c r="E3" s="1">
-        <v>2001</v>
-      </c>
-      <c r="F3" s="1">
-        <v>2002</v>
-      </c>
-      <c r="G3" s="1">
-        <v>2003</v>
-      </c>
-      <c r="H3" s="1">
-        <v>2004</v>
-      </c>
-      <c r="I3" s="1">
-        <v>2005</v>
-      </c>
-      <c r="J3" s="1">
-        <v>2006</v>
-      </c>
-      <c r="K3" s="1">
-        <v>2007</v>
-      </c>
-      <c r="L3" s="1">
-        <v>2008</v>
-      </c>
-      <c r="M3" s="1">
-        <v>2009</v>
-      </c>
-      <c r="N3" s="1">
-        <v>2010</v>
-      </c>
-      <c r="O3" s="1">
-        <v>2011</v>
-      </c>
-      <c r="P3" s="1">
-        <v>2012</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>2013</v>
-      </c>
-      <c r="R3" s="1">
-        <v>2014</v>
-      </c>
-      <c r="S3" s="1">
-        <v>2015</v>
-      </c>
-      <c r="T3" s="1">
-        <v>2016</v>
-      </c>
-      <c r="U3" s="1">
-        <v>2017</v>
-      </c>
-      <c r="V3" s="1">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1">
-        <v>2000</v>
-      </c>
-      <c r="E5" s="1">
-        <v>2001</v>
-      </c>
-      <c r="F5" s="1">
-        <v>2002</v>
-      </c>
-      <c r="G5" s="1">
-        <v>2003</v>
-      </c>
-      <c r="H5" s="1">
-        <v>2004</v>
-      </c>
-      <c r="I5" s="1">
-        <v>2005</v>
-      </c>
-      <c r="J5" s="1">
-        <v>2006</v>
-      </c>
-      <c r="K5" s="1">
-        <v>2007</v>
-      </c>
-      <c r="L5" s="1">
-        <v>2008</v>
-      </c>
-      <c r="M5" s="1">
-        <v>2009</v>
-      </c>
-      <c r="N5" s="1">
-        <v>2010</v>
-      </c>
-      <c r="O5" s="1">
-        <v>2011</v>
-      </c>
-      <c r="P5" s="1">
-        <v>2012</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>2013</v>
-      </c>
-      <c r="R5" s="1">
-        <v>2014</v>
-      </c>
-      <c r="S5" s="1">
-        <v>2015</v>
-      </c>
-      <c r="T5" s="1">
-        <v>2016</v>
-      </c>
-      <c r="U5" s="1">
-        <v>2017</v>
-      </c>
-      <c r="V5" s="1">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>8</v>
@@ -1309,9 +1314,9 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>8</v>
@@ -1374,9 +1379,9 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>8</v>
@@ -1436,6 +1441,136 @@
         <v>2017</v>
       </c>
       <c r="V11" s="1">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="1">
+        <v>2000</v>
+      </c>
+      <c r="E13" s="1">
+        <v>2001</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2002</v>
+      </c>
+      <c r="G13" s="1">
+        <v>2003</v>
+      </c>
+      <c r="H13" s="1">
+        <v>2004</v>
+      </c>
+      <c r="I13" s="1">
+        <v>2005</v>
+      </c>
+      <c r="J13" s="1">
+        <v>2006</v>
+      </c>
+      <c r="K13" s="1">
+        <v>2007</v>
+      </c>
+      <c r="L13" s="1">
+        <v>2008</v>
+      </c>
+      <c r="M13" s="1">
+        <v>2009</v>
+      </c>
+      <c r="N13" s="1">
+        <v>2010</v>
+      </c>
+      <c r="O13" s="1">
+        <v>2011</v>
+      </c>
+      <c r="P13" s="1">
+        <v>2012</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>2013</v>
+      </c>
+      <c r="R13" s="1">
+        <v>2014</v>
+      </c>
+      <c r="S13" s="1">
+        <v>2015</v>
+      </c>
+      <c r="T13" s="1">
+        <v>2016</v>
+      </c>
+      <c r="U13" s="1">
+        <v>2017</v>
+      </c>
+      <c r="V13" s="1">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2000</v>
+      </c>
+      <c r="E15" s="1">
+        <v>2001</v>
+      </c>
+      <c r="F15" s="1">
+        <v>2002</v>
+      </c>
+      <c r="G15" s="1">
+        <v>2003</v>
+      </c>
+      <c r="H15" s="1">
+        <v>2004</v>
+      </c>
+      <c r="I15" s="1">
+        <v>2005</v>
+      </c>
+      <c r="J15" s="1">
+        <v>2006</v>
+      </c>
+      <c r="K15" s="1">
+        <v>2007</v>
+      </c>
+      <c r="L15" s="1">
+        <v>2008</v>
+      </c>
+      <c r="M15" s="1">
+        <v>2009</v>
+      </c>
+      <c r="N15" s="1">
+        <v>2010</v>
+      </c>
+      <c r="O15" s="1">
+        <v>2011</v>
+      </c>
+      <c r="P15" s="1">
+        <v>2012</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>2013</v>
+      </c>
+      <c r="R15" s="1">
+        <v>2014</v>
+      </c>
+      <c r="S15" s="1">
+        <v>2015</v>
+      </c>
+      <c r="T15" s="1">
+        <v>2016</v>
+      </c>
+      <c r="U15" s="1">
+        <v>2017</v>
+      </c>
+      <c r="V15" s="1">
         <v>2018</v>
       </c>
     </row>
@@ -1446,20 +1581,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:V20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="50.6640625" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -1524,7 +1659,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="str">
         <f>'Population Definitions'!B2</f>
         <v>Adults</v>
@@ -1536,7 +1671,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -1601,7 +1736,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="str">
         <f>'Population Definitions'!B2</f>
         <v>Adults</v>
@@ -1614,7 +1749,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -1679,7 +1814,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="str">
         <f>'Population Definitions'!B2</f>
         <v>Adults</v>
@@ -1692,7 +1827,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -1757,7 +1892,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="str">
         <f>'Population Definitions'!B2</f>
         <v>Adults</v>
@@ -1770,7 +1905,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -1835,7 +1970,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="str">
         <f>'Population Definitions'!B2</f>
         <v>Adults</v>
@@ -1848,7 +1983,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -1913,7 +2048,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="str">
         <f>'Population Definitions'!B2</f>
         <v>Adults</v>
@@ -1926,7 +2061,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -1991,7 +2126,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="str">
         <f>'Population Definitions'!B2</f>
         <v>Adults</v>

</xml_diff>

<commit_message>
Compartments hacked into parameter set
Compartments now act like characteristics, in that they can be associated with user-provided values in Project.data and, via propagation, Project.parsets.
However, these parameter set values are only ever used in initialising the model, during which actual compartment sizes are calculated via linear algebra methods.
The SIR test for model setup in old and improved Optima TB is now functional.
The next step is to ensure dynamics are operating properly by considering relative/absolute formats.
</commit_message>
<xml_diff>
--- a/tests/databooks/databook_sir.xlsx
+++ b/tests/databooks/databook_sir.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects - Work\Optima\atomica\tests\databooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3F6859-C6A2-41D7-95DE-DED3A0A63504}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA422128-FA78-4F45-ADD4-4405EADEF000}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="13440" windowHeight="9660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Population Definitions" sheetId="1" r:id="rId1"/>
@@ -853,7 +853,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -937,8 +937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:V8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
SIR cleaned and tweaked
Got rid of the initial prevalence parameter and made FOI directly dependent on prevalence (i.e. nonlinear).
Also increased duration of infection to slow down recovery rate and increased transmission probability to boost FOI, thus avoiding the immediate disappearance of the epidemic.
Deaths increase at a faster pace early on when there is a pulse of infections, but slows down as people recover.
</commit_message>
<xml_diff>
--- a/tests/databooks/databook_sir.xlsx
+++ b/tests/databooks/databook_sir.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects - Work\Optima\atomica\tests\databooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{63B041D6-5198-4DC8-8263-28BB23A028B9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E51E2250-94CD-4669-B3D5-B2B621BDB874}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -382,7 +382,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000A000000}">
+    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -395,7 +395,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000B000000}">
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -409,7 +409,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{350FA826-1034-4FED-9BB0-CF8AEC055305}">
+    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{A34E5756-14AC-4CA6-8F9C-29CFA0AA4A59}">
       <text>
         <r>
           <rPr>
@@ -426,7 +426,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000D000000}">
+    <comment ref="A13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000010000000}">
       <text>
         <r>
           <rPr>
@@ -439,7 +439,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000E000000}">
+    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000011000000}">
       <text>
         <r>
           <rPr>
@@ -453,7 +453,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{A34E5756-14AC-4CA6-8F9C-29CFA0AA4A59}">
+    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{E22C0B53-AFF3-4BC4-88F2-74A45EA18B1D}">
       <text>
         <r>
           <rPr>
@@ -470,56 +470,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="A16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000010000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This is a parameter.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000011000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column displays the type of quantity that the databook is requesting, e.g. probability, duration, number, etc.
-In some cases, the user may select the format for the data, to align with data collection pragmatics, and appropriate conversions will be done internally to the model.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C16" authorId="0" shapeId="0" xr:uid="{E22C0B53-AFF3-4BC4-88F2-74A45EA18B1D}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column should be filled with default values used by the model.
-If the option to provide time-dependent values exists, then this can be considered a time-independent assumption.
-In this case, if any time-dependent values are entered, the Excel sheet will attempt to explicitly mark the corresponding cell as inapplicable.
-Alternatively, the user can leave the cell blank.
-However, any other value will override the time-dependent values during a model run.</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="25">
   <si>
     <t>Abbreviation</t>
   </si>
@@ -582,9 +538,6 @@
   </si>
   <si>
     <t>Death rate for infected people</t>
-  </si>
-  <si>
-    <t>Initial prevalence</t>
   </si>
   <si>
     <t>Transmission probability per contact</t>
@@ -1013,10 +966,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1357,10 +1310,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:W17"/>
+  <dimension ref="A1:W14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1531,8 +1484,7 @@
         <v>19</v>
       </c>
       <c r="C5">
-        <f>IF(SUMPRODUCT(--(E5:W5&lt;&gt;""))=0,0.5,"N.A.")</f>
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>12</v>
@@ -1699,8 +1651,7 @@
         <v>17</v>
       </c>
       <c r="C11">
-        <f>IF(SUMPRODUCT(--(E11:W11&lt;&gt;""))=0,0.005,"N.A.")</f>
-        <v>5.0000000000000001E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>12</v>
@@ -1780,118 +1731,25 @@
         <v>Adults</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C14">
-        <f>IF(SUMPRODUCT(--(E14:W14&lt;&gt;""))=0,0.0008,"N.A.")</f>
-        <v>8.0000000000000004E-4</v>
+        <f>IF(SUMPRODUCT(--(E14:W14&lt;&gt;""))=0,80,"N.A.")</f>
+        <v>80</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="1">
-        <v>2000</v>
-      </c>
-      <c r="F16" s="1">
-        <v>2001</v>
-      </c>
-      <c r="G16" s="1">
-        <v>2002</v>
-      </c>
-      <c r="H16" s="1">
-        <v>2003</v>
-      </c>
-      <c r="I16" s="1">
-        <v>2004</v>
-      </c>
-      <c r="J16" s="1">
-        <v>2005</v>
-      </c>
-      <c r="K16" s="1">
-        <v>2006</v>
-      </c>
-      <c r="L16" s="1">
-        <v>2007</v>
-      </c>
-      <c r="M16" s="1">
-        <v>2008</v>
-      </c>
-      <c r="N16" s="1">
-        <v>2009</v>
-      </c>
-      <c r="O16" s="1">
-        <v>2010</v>
-      </c>
-      <c r="P16" s="1">
-        <v>2011</v>
-      </c>
-      <c r="Q16" s="1">
-        <v>2012</v>
-      </c>
-      <c r="R16" s="1">
-        <v>2013</v>
-      </c>
-      <c r="S16" s="1">
-        <v>2014</v>
-      </c>
-      <c r="T16" s="1">
-        <v>2015</v>
-      </c>
-      <c r="U16" s="1">
-        <v>2016</v>
-      </c>
-      <c r="V16" s="1">
-        <v>2017</v>
-      </c>
-      <c r="W16" s="1">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A17" s="2" t="str">
-        <f>'Population Definitions'!B2</f>
-        <v>Adults</v>
-      </c>
-      <c r="B17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17">
-        <f>IF(SUMPRODUCT(--(E17:W17&lt;&gt;""))=0,80,"N.A.")</f>
-        <v>80</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
   </sheetData>
-  <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{00000000-0002-0000-0300-000000000000}">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B11 B8" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"Probability"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>"Duration"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8" xr:uid="{00000000-0002-0000-0300-000002000000}">
-      <formula1>"Probability"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11" xr:uid="{00000000-0002-0000-0300-000003000000}">
-      <formula1>"Probability"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B14" xr:uid="{00000000-0002-0000-0300-000004000000}">
-      <formula1>"Probability"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17" xr:uid="{00000000-0002-0000-0300-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B14" xr:uid="{00000000-0002-0000-0300-000005000000}">
       <formula1>"Number"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added project data time values and refactored TimeSeries
</commit_message>
<xml_diff>
--- a/tests/databooks/databook_sir.xlsx
+++ b/tests/databooks/databook_sir.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects - Work\Optima\atomica\tests\databooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romesh.abey\Desktop\projects\atomica\atomica\tests\databooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E51E2250-94CD-4669-B3D5-B2B621BDB874}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="18" windowWidth="16098" windowHeight="9660" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Population Definitions" sheetId="1" r:id="rId1"/>
@@ -18,17 +17,17 @@
     <sheet name="State Variables" sheetId="3" r:id="rId3"/>
     <sheet name="Parameters" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -43,7 +42,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -63,12 +62,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -83,7 +82,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -103,12 +102,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -121,7 +120,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -135,7 +134,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -152,7 +151,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
+    <comment ref="A4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -165,7 +164,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
+    <comment ref="B4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -179,7 +178,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000006000000}">
+    <comment ref="C4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -196,7 +195,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000007000000}">
+    <comment ref="A7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -209,7 +208,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000008000000}">
+    <comment ref="B7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -223,7 +222,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000009000000}">
+    <comment ref="C7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -245,12 +244,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -263,7 +262,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -277,7 +276,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{B4D16957-06E8-4BFF-9F93-D3562E084FF1}">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -294,7 +293,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
+    <comment ref="A4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -307,7 +306,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000005000000}">
+    <comment ref="B4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -321,7 +320,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{59555E9E-5921-4B84-B52C-B8210DFCACB0}">
+    <comment ref="C4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -338,7 +337,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000007000000}">
+    <comment ref="A7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -351,7 +350,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000008000000}">
+    <comment ref="B7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -365,7 +364,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{DE05BA36-86E1-4F22-8B5D-5294D5590975}">
+    <comment ref="C7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -382,7 +381,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000D000000}">
+    <comment ref="A10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -395,7 +394,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000E000000}">
+    <comment ref="B10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -409,7 +408,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{A34E5756-14AC-4CA6-8F9C-29CFA0AA4A59}">
+    <comment ref="C10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -426,7 +425,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000010000000}">
+    <comment ref="A13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -439,7 +438,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000011000000}">
+    <comment ref="B13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -453,7 +452,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{E22C0B53-AFF3-4BC4-88F2-74A45EA18B1D}">
+    <comment ref="C13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -475,7 +474,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
   <si>
     <t>Abbreviation</t>
   </si>
@@ -555,7 +554,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -700,23 +699,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -752,23 +734,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -944,19 +909,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="2" width="15.73046875" customWidth="1"/>
+    <col min="1" max="2" width="15.734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -964,7 +929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
@@ -979,17 +944,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="2" width="20.73046875" customWidth="1"/>
+    <col min="1" max="2" width="20.734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -997,7 +962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1005,7 +970,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1013,7 +978,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1028,21 +993,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="50.73046875" customWidth="1"/>
-    <col min="2" max="2" width="15.73046875" customWidth="1"/>
-    <col min="3" max="3" width="10.73046875" customWidth="1"/>
+    <col min="1" max="1" width="20.41796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.734375" customWidth="1"/>
+    <col min="3" max="3" width="10.734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1110,7 +1075,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="str">
         <f>'Population Definitions'!B2</f>
         <v>Adults</v>
@@ -1125,7 +1090,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -1193,7 +1158,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="str">
         <f>'Population Definitions'!B2</f>
         <v>Adults</v>
@@ -1208,7 +1173,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -1276,30 +1241,35 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A8" s="2" t="str">
-        <f>'Population Definitions'!B2</f>
-        <v>Adults</v>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
       </c>
-      <c r="C8">
-        <v>0.2</v>
-      </c>
       <c r="D8" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="E8">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="J8">
+        <v>1.2740740740740741</v>
+      </c>
+      <c r="O8">
+        <v>2.4456521739130435</v>
+      </c>
+      <c r="T8">
+        <v>0.27083333333333331</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{00000000-0002-0000-0200-000000000000}">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B5">
       <formula1>"Number"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0200-000001000000}">
-      <formula1>"Number"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8" xr:uid="{00000000-0002-0000-0200-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8">
       <formula1>"Fraction"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1309,21 +1279,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="50.73046875" customWidth="1"/>
-    <col min="2" max="2" width="15.73046875" customWidth="1"/>
-    <col min="3" max="3" width="10.73046875" customWidth="1"/>
+    <col min="1" max="1" width="50.734375" customWidth="1"/>
+    <col min="2" max="2" width="15.734375" customWidth="1"/>
+    <col min="3" max="3" width="10.734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -1391,7 +1361,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="str">
         <f>'Population Definitions'!B2</f>
         <v>Adults</v>
@@ -1407,7 +1377,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -1475,7 +1445,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="str">
         <f>'Population Definitions'!B2</f>
         <v>Adults</v>
@@ -1490,7 +1460,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -1558,7 +1528,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="str">
         <f>'Population Definitions'!B2</f>
         <v>Adults</v>
@@ -1574,7 +1544,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
@@ -1642,7 +1612,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="str">
         <f>'Population Definitions'!B2</f>
         <v>Adults</v>
@@ -1657,7 +1627,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -1725,7 +1695,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2" t="str">
         <f>'Population Definitions'!B2</f>
         <v>Adults</v>
@@ -1743,13 +1713,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B11 B8" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B11 B8">
       <formula1>"Probability"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0300-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
       <formula1>"Duration"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B14" xr:uid="{00000000-0002-0000-0300-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B14">
       <formula1>"Number"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Updated databook calibration values
</commit_message>
<xml_diff>
--- a/tests/databooks/databook_sir.xlsx
+++ b/tests/databooks/databook_sir.xlsx
@@ -996,8 +996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AC6" sqref="AC6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1248,20 +1248,68 @@
       <c r="B8" t="s">
         <v>15</v>
       </c>
+      <c r="C8">
+        <v>0.2</v>
+      </c>
       <c r="D8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E8">
-        <v>0.2857142857142857</v>
+        <v>0.28571428999999998</v>
+      </c>
+      <c r="F8">
+        <v>0.25792055000000003</v>
+      </c>
+      <c r="G8">
+        <v>0.23218095999999999</v>
+      </c>
+      <c r="H8">
+        <v>0.20849680000000001</v>
+      </c>
+      <c r="I8">
+        <v>0.18682389999999999</v>
       </c>
       <c r="J8">
-        <v>1.2740740740740741</v>
+        <v>0.16708539</v>
+      </c>
+      <c r="K8">
+        <v>0.14918208999999999</v>
+      </c>
+      <c r="L8">
+        <v>0.13300081999999999</v>
+      </c>
+      <c r="M8">
+        <v>0.11842081</v>
+      </c>
+      <c r="N8">
+        <v>0.10531865999999999</v>
       </c>
       <c r="O8">
-        <v>2.4456521739130435</v>
+        <v>9.3571909999999994E-2</v>
+      </c>
+      <c r="P8">
+        <v>8.3061700000000002E-2</v>
+      </c>
+      <c r="Q8">
+        <v>7.3674489999999995E-2</v>
+      </c>
+      <c r="R8">
+        <v>6.5303260000000002E-2</v>
+      </c>
+      <c r="S8">
+        <v>5.7848160000000003E-2</v>
       </c>
       <c r="T8">
-        <v>0.27083333333333331</v>
+        <v>5.1216810000000002E-2</v>
+      </c>
+      <c r="U8">
+        <v>4.5324320000000001E-2</v>
+      </c>
+      <c r="V8">
+        <v>4.0093150000000001E-2</v>
+      </c>
+      <c r="W8">
+        <v>3.54528E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor databook ordering fix
Workbook table parsing is currently rigidly in the order that table objects are generated in the corresponding page specifications.
This rigidity should be corrected, but, for now, tables must be ordered appropriately.
With this fix, the SIR test case works fine, allowing both the test and api script to flow without problem.
</commit_message>
<xml_diff>
--- a/tests/databooks/databook_sir.xlsx
+++ b/tests/databooks/databook_sir.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romesh.abey\Desktop\projects\atomica\atomica\tests\databooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects - Work\Optima\atomica\tests\databooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37E9D1B-BD18-4DA4-BC87-538628FCE450}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="18" windowWidth="16098" windowHeight="9660" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Population Definitions" sheetId="1" r:id="rId1"/>
@@ -17,17 +18,17 @@
     <sheet name="State Variables" sheetId="3" r:id="rId3"/>
     <sheet name="Parameters" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -42,7 +43,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -62,12 +63,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -82,7 +83,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -102,12 +103,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -120,7 +121,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -134,7 +135,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -151,7 +152,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0" shapeId="0">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
       <text>
         <r>
           <rPr>
@@ -164,7 +165,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0" shapeId="0">
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
       <text>
         <r>
           <rPr>
@@ -178,7 +179,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C4" authorId="0" shapeId="0">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000006000000}">
       <text>
         <r>
           <rPr>
@@ -195,7 +196,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0">
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000007000000}">
       <text>
         <r>
           <rPr>
@@ -208,7 +209,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0" shapeId="0">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000008000000}">
       <text>
         <r>
           <rPr>
@@ -222,7 +223,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C7" authorId="0" shapeId="0">
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000009000000}">
       <text>
         <r>
           <rPr>
@@ -244,12 +245,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -262,7 +263,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -276,7 +277,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -293,7 +294,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0" shapeId="0">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -306,7 +307,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0" shapeId="0">
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -320,7 +321,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C4" authorId="0" shapeId="0">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -337,7 +338,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0">
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
       <text>
         <r>
           <rPr>
@@ -350,7 +351,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0" shapeId="0">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000005000000}">
       <text>
         <r>
           <rPr>
@@ -364,7 +365,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C7" authorId="0" shapeId="0">
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000006000000}">
       <text>
         <r>
           <rPr>
@@ -381,7 +382,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A10" authorId="0" shapeId="0">
+    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000007000000}">
       <text>
         <r>
           <rPr>
@@ -394,7 +395,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="0" shapeId="0">
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000008000000}">
       <text>
         <r>
           <rPr>
@@ -408,7 +409,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C10" authorId="0" shapeId="0">
+    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000009000000}">
       <text>
         <r>
           <rPr>
@@ -425,7 +426,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A13" authorId="0" shapeId="0">
+    <comment ref="A13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -438,7 +439,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B13" authorId="0" shapeId="0">
+    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -452,7 +453,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C13" authorId="0" shapeId="0">
+    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
       <text>
         <r>
           <rPr>
@@ -554,7 +555,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -699,6 +700,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -734,6 +752,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -909,19 +944,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="2" width="15.734375" customWidth="1"/>
+    <col min="1" max="2" width="15.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -929,7 +964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
@@ -944,17 +979,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="2" width="20.734375" customWidth="1"/>
+    <col min="1" max="2" width="20.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -962,7 +997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -970,7 +1005,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -978,7 +1013,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -993,21 +1028,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:W8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AC6" sqref="AC6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="20.41796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.734375" customWidth="1"/>
-    <col min="3" max="3" width="10.734375" customWidth="1"/>
+    <col min="1" max="1" width="20.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.73046875" customWidth="1"/>
+    <col min="3" max="3" width="10.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1075,7 +1110,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="str">
         <f>'Population Definitions'!B2</f>
         <v>Adults</v>
@@ -1090,7 +1125,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -1158,7 +1193,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="str">
         <f>'Population Definitions'!B2</f>
         <v>Adults</v>
@@ -1173,7 +1208,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -1241,7 +1276,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
@@ -1314,10 +1349,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B5" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Number"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"Fraction"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1327,23 +1362,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:W14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="50.734375" customWidth="1"/>
-    <col min="2" max="2" width="15.734375" customWidth="1"/>
-    <col min="3" max="3" width="10.734375" customWidth="1"/>
+    <col min="1" max="1" width="50.73046875" customWidth="1"/>
+    <col min="2" max="2" width="15.73046875" customWidth="1"/>
+    <col min="3" max="3" width="10.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>9</v>
@@ -1409,7 +1444,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="str">
         <f>'Population Definitions'!B2</f>
         <v>Adults</v>
@@ -1418,16 +1453,15 @@
         <v>17</v>
       </c>
       <c r="C2">
-        <f>IF(SUMPRODUCT(--(E2:W2&lt;&gt;""))=0,0.008,"N.A.")</f>
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
@@ -1493,24 +1527,25 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="str">
         <f>'Population Definitions'!B2</f>
         <v>Adults</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <f>IF(SUMPRODUCT(--(E5:W5&lt;&gt;""))=0,80,"N.A.")</f>
+        <v>80</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>9</v>
@@ -1576,25 +1611,24 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="str">
         <f>'Population Definitions'!B2</f>
         <v>Adults</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C8">
-        <f>IF(SUMPRODUCT(--(E8:W8&lt;&gt;""))=0,0.016,"N.A.")</f>
-        <v>1.6E-2</v>
+        <v>5</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>9</v>
@@ -1660,7 +1694,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="str">
         <f>'Population Definitions'!B2</f>
         <v>Adults</v>
@@ -1669,15 +1703,16 @@
         <v>17</v>
       </c>
       <c r="C11">
-        <v>8.0000000000000002E-3</v>
+        <f>IF(SUMPRODUCT(--(E11:W11&lt;&gt;""))=0,0.016,"N.A.")</f>
+        <v>1.6E-2</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>9</v>
@@ -1743,17 +1778,17 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="str">
         <f>'Population Definitions'!B2</f>
         <v>Adults</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C14">
-        <f>IF(SUMPRODUCT(--(E14:W14&lt;&gt;""))=0,80,"N.A.")</f>
-        <v>80</v>
+        <f>IF(SUMPRODUCT(--(E14:W14&lt;&gt;""))=0,0.008,"N.A.")</f>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>12</v>
@@ -1761,13 +1796,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B11 B8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B14 B2 B11" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"Probability"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>"Duration"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0300-000002000000}">
       <formula1>"Number"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Testing that duration format works
SIR databook updated with transfer sheets, just to make sure that duration format is handled properly by model iterations via test script.
</commit_message>
<xml_diff>
--- a/tests/databooks/databook_sir.xlsx
+++ b/tests/databooks/databook_sir.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects - Work\Optima\atomica\tests\databooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37E9D1B-BD18-4DA4-BC87-538628FCE450}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B6A38B-2BCD-4628-B103-FFA0941AF75B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Population Definitions" sheetId="1" r:id="rId1"/>
-    <sheet name="Program Definitions" sheetId="2" r:id="rId2"/>
-    <sheet name="State Variables" sheetId="3" r:id="rId3"/>
-    <sheet name="Parameters" sheetId="4" r:id="rId4"/>
+    <sheet name="Transfer Definitions" sheetId="5" r:id="rId2"/>
+    <sheet name="Transfer Details" sheetId="6" r:id="rId3"/>
+    <sheet name="Program Definitions" sheetId="2" r:id="rId4"/>
+    <sheet name="State Variables" sheetId="3" r:id="rId5"/>
+    <sheet name="Parameters" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="179017"/>
 </workbook>
@@ -68,32 +70,49 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column is for the abbreviated name of a population.
-It is only ever used as a reference label within the code.
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{E7F6C3C7-0FE9-44E6-86E9-9DFFE65D74B6}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column is for the abbreviated name of a transfer.
+A transfer is a movement of entities between populations,
+which, by default, is from compartment to corresponding
+compartment.
+The flow number is, by default, distributed in proportion
+to the size of all compartments in the source population.
+A common example is 'aging', where a specified fraction of
+people in one age bracket move per year to the next age
+bracket.
+The abbreviation is only ever used as a reference label
+within the code.
 Note: It should be in lower case without spaces.</t>
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column is for the full name of a program.
-It will appear in plots and analysis outputs.
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{1C309BE7-3A33-4B27-818D-F7B2A7B2DA0C}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column is for the full name of a transfer.
+A transfer is a movement of entities between populations,
+which, by default, is from compartment to corresponding
+compartment.
+The flow number is, by default, distributed in proportion
+to the size of all compartments in the source population.
+A common example is 'Aging', where a specified fraction of
+people in one age bracket move per year to the next age
+bracket.
+The full name will appear in plots and analysis outputs.
 Note: It should be in title or sentence case.</t>
         </r>
       </text>
@@ -108,20 +127,30 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column defines a 'label' attribute for a 'comp' item.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{72944053-F456-4F94-9F8B-FF737E24577E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column is for the full name of a transfer.
+A transfer is a movement of entities between populations,
+which, by default, is from compartment to corresponding
+compartment.
+The flow number is, by default, distributed in proportion
+to the size of all compartments in the source population.
+A common example is 'Aging', where a specified fraction of
+people in one age bracket move per year to the next age
+bracket.
+The full name will appear in plots and analysis outputs.
+Note: It should be in title or sentence case.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{37B0BB7D-4D79-4DFA-90C6-6D2E0BD5A184}">
       <text>
         <r>
           <rPr>
@@ -135,95 +164,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column should be filled with default values used by the model.
-If the option to provide time-dependent values exists, then this can be considered a time-independent assumption.
-In this case, if any time-dependent values are entered, the Excel sheet will attempt to explicitly mark the corresponding cell as inapplicable.
-Alternatively, the user can leave the cell blank.
-However, any other value will override the time-dependent values during a model run.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This is a characteristic.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column displays the type of quantity that the databook is requesting, e.g. probability, duration, number, etc.
-In some cases, the user may select the format for the data, to align with data collection pragmatics, and appropriate conversions will be done internally to the model.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000006000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column should be filled with default values used by the model.
-If the option to provide time-dependent values exists, then this can be considered a time-independent assumption.
-In this case, if any time-dependent values are entered, the Excel sheet will attempt to explicitly mark the corresponding cell as inapplicable.
-Alternatively, the user can leave the cell blank.
-However, any other value will override the time-dependent values during a model run.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000007000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This is a characteristic.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000008000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column displays the type of quantity that the databook is requesting, e.g. probability, duration, number, etc.
-In some cases, the user may select the format for the data, to align with data collection pragmatics, and appropriate conversions will be done internally to the model.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000009000000}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{7F3CF7F1-9D77-4CAE-B0F7-A9240FC1E148}">
       <text>
         <r>
           <rPr>
@@ -250,20 +191,60 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000A000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This is a parameter.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000B000000}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column is for the abbreviated name of a population.
+It is only ever used as a reference label within the code.
+Note: It should be in lower case without spaces.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column is for the full name of a program.
+It will appear in plots and analysis outputs.
+Note: It should be in title or sentence case.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column defines a 'label' attribute for a 'comp' item.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -277,7 +258,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000C000000}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -294,20 +275,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000D000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This is a parameter.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000E000000}">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is a characteristic.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
       <text>
         <r>
           <rPr>
@@ -321,7 +302,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000F000000}">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000006000000}">
       <text>
         <r>
           <rPr>
@@ -338,20 +319,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This is a parameter.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000005000000}">
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000007000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is a characteristic.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000008000000}">
       <text>
         <r>
           <rPr>
@@ -365,7 +346,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000006000000}">
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000009000000}">
       <text>
         <r>
           <rPr>
@@ -382,7 +363,17 @@
         </r>
       </text>
     </comment>
-    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000007000000}">
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -395,7 +386,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000008000000}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -409,7 +400,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000009000000}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -426,7 +417,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -439,7 +430,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -453,7 +444,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -470,12 +461,144 @@
         </r>
       </text>
     </comment>
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is a parameter.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000005000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column displays the type of quantity that the databook is requesting, e.g. probability, duration, number, etc.
+In some cases, the user may select the format for the data, to align with data collection pragmatics, and appropriate conversions will be done internally to the model.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000006000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column should be filled with default values used by the model.
+If the option to provide time-dependent values exists, then this can be considered a time-independent assumption.
+In this case, if any time-dependent values are entered, the Excel sheet will attempt to explicitly mark the corresponding cell as inapplicable.
+Alternatively, the user can leave the cell blank.
+However, any other value will override the time-dependent values during a model run.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000007000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is a parameter.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000008000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column displays the type of quantity that the databook is requesting, e.g. probability, duration, number, etc.
+In some cases, the user may select the format for the data, to align with data collection pragmatics, and appropriate conversions will be done internally to the model.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000009000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column should be filled with default values used by the model.
+If the option to provide time-dependent values exists, then this can be considered a time-independent assumption.
+In this case, if any time-dependent values are entered, the Excel sheet will attempt to explicitly mark the corresponding cell as inapplicable.
+Alternatively, the user can leave the cell blank.
+However, any other value will override the time-dependent values during a model run.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is a parameter.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column displays the type of quantity that the databook is requesting, e.g. probability, duration, number, etc.
+In some cases, the user may select the format for the data, to align with data collection pragmatics, and appropriate conversions will be done internally to the model.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column should be filled with default values used by the model.
+If the option to provide time-dependent values exists, then this can be considered a time-independent assumption.
+In this case, if any time-dependent values are entered, the Excel sheet will attempt to explicitly mark the corresponding cell as inapplicable.
+Alternatively, the user can leave the cell blank.
+However, any other value will override the time-dependent values during a model run.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="28">
   <si>
     <t>Abbreviation</t>
   </si>
@@ -550,6 +673,15 @@
   </si>
   <si>
     <t>Adults</t>
+  </si>
+  <si>
+    <t>trans_0</t>
+  </si>
+  <si>
+    <t>Transfer 0</t>
+  </si>
+  <si>
+    <t>N.A.</t>
   </si>
 </sst>
 </file>
@@ -979,6 +1111,144 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8173DB03-9DA9-4723-BA4D-D4F2E4218144}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="2" width="15.73046875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="str">
+        <f>$B$2</f>
+        <v>Transfer 0</v>
+      </c>
+      <c r="B4" s="1" t="str">
+        <f>'Population Definitions'!$A$2</f>
+        <v>adults</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="str">
+        <f>'Population Definitions'!$A$2</f>
+        <v>adults</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{845C5B9F-F956-439D-BFEE-D0A4DBEE719E}">
+      <formula1>"N.A."</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B99B07ED-0F90-40C4-B349-276E5F4A7E2B}">
+  <dimension ref="A1:V1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="15.73046875" customWidth="1"/>
+    <col min="4" max="4" width="15.73046875" customWidth="1"/>
+    <col min="5" max="5" width="10.73046875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="str">
+        <f>'Transfer Definitions'!$B$2</f>
+        <v>Transfer 0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2000</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2001</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2002</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2003</v>
+      </c>
+      <c r="K1" s="1">
+        <v>2004</v>
+      </c>
+      <c r="L1" s="1">
+        <v>2005</v>
+      </c>
+      <c r="M1" s="1">
+        <v>2006</v>
+      </c>
+      <c r="N1" s="1">
+        <v>2007</v>
+      </c>
+      <c r="O1" s="1">
+        <v>2008</v>
+      </c>
+      <c r="P1" s="1">
+        <v>2009</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>2010</v>
+      </c>
+      <c r="R1" s="1">
+        <v>2011</v>
+      </c>
+      <c r="S1" s="1">
+        <v>2012</v>
+      </c>
+      <c r="T1" s="1">
+        <v>2013</v>
+      </c>
+      <c r="U1" s="1">
+        <v>2014</v>
+      </c>
+      <c r="V1" s="1">
+        <v>2015</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1027,7 +1297,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:W8"/>
   <sheetViews>
@@ -1361,11 +1631,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:W14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Working data plots on single cascade
</commit_message>
<xml_diff>
--- a/tests/databooks/databook_sir.xlsx
+++ b/tests/databooks/databook_sir.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\tests\databooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34224A1-2122-4354-A928-5650BC9D8660}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{241EE670-F775-4CB1-A4B7-6CBC2C0BCEB0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Population Definitions" sheetId="1" r:id="rId1"/>
     <sheet name="State Variables" sheetId="3" r:id="rId2"/>
     <sheet name="Parameters" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
@@ -923,8 +923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:W8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1010,11 +1010,65 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2">
-        <v>700</v>
-      </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="E2">
+        <v>700</v>
+      </c>
+      <c r="F2">
+        <v>700</v>
+      </c>
+      <c r="G2">
+        <v>700</v>
+      </c>
+      <c r="H2">
+        <v>700</v>
+      </c>
+      <c r="I2">
+        <v>700</v>
+      </c>
+      <c r="J2">
+        <v>700</v>
+      </c>
+      <c r="K2">
+        <v>700</v>
+      </c>
+      <c r="L2">
+        <v>700</v>
+      </c>
+      <c r="M2">
+        <v>700</v>
+      </c>
+      <c r="N2">
+        <v>700</v>
+      </c>
+      <c r="O2">
+        <v>700</v>
+      </c>
+      <c r="P2">
+        <v>700</v>
+      </c>
+      <c r="Q2">
+        <v>700</v>
+      </c>
+      <c r="R2">
+        <v>700</v>
+      </c>
+      <c r="S2">
+        <v>700</v>
+      </c>
+      <c r="T2">
+        <v>700</v>
+      </c>
+      <c r="U2">
+        <v>700</v>
+      </c>
+      <c r="V2">
+        <v>700</v>
+      </c>
+      <c r="W2">
+        <v>700</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
@@ -1093,11 +1147,65 @@
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5">
-        <v>1000</v>
-      </c>
       <c r="D5" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="E5">
+        <v>1000</v>
+      </c>
+      <c r="F5">
+        <v>1000</v>
+      </c>
+      <c r="G5">
+        <v>1000</v>
+      </c>
+      <c r="H5">
+        <v>1000</v>
+      </c>
+      <c r="I5">
+        <v>1000</v>
+      </c>
+      <c r="J5">
+        <v>1000</v>
+      </c>
+      <c r="K5">
+        <v>1000</v>
+      </c>
+      <c r="L5">
+        <v>1000</v>
+      </c>
+      <c r="M5">
+        <v>1000</v>
+      </c>
+      <c r="N5">
+        <v>1000</v>
+      </c>
+      <c r="O5">
+        <v>1000</v>
+      </c>
+      <c r="P5">
+        <v>1000</v>
+      </c>
+      <c r="Q5">
+        <v>1000</v>
+      </c>
+      <c r="R5">
+        <v>1000</v>
+      </c>
+      <c r="S5">
+        <v>1000</v>
+      </c>
+      <c r="T5">
+        <v>1000</v>
+      </c>
+      <c r="U5">
+        <v>1000</v>
+      </c>
+      <c r="V5">
+        <v>1000</v>
+      </c>
+      <c r="W5">
+        <v>1000</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
@@ -1175,9 +1283,6 @@
       </c>
       <c r="B8" t="s">
         <v>9</v>
-      </c>
-      <c r="C8">
-        <v>0.2</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>6</v>
@@ -1258,7 +1363,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:W14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update SIR, check that it works
</commit_message>
<xml_diff>
--- a/tests/databooks/databook_sir.xlsx
+++ b/tests/databooks/databook_sir.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\tests\databooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53FC4FC7-BDB6-4C27-9510-84F52D8A3C97}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C3639E-3B58-4F47-84FF-F34919B62B05}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,6 +18,13 @@
     <sheet name="Parameters" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179021"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -434,7 +441,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="20">
   <si>
     <t>Abbreviation</t>
   </si>
@@ -491,6 +498,9 @@
   </si>
   <si>
     <t>Units</t>
+  </si>
+  <si>
+    <t>N.A.</t>
   </si>
 </sst>
 </file>
@@ -1364,7 +1374,7 @@
   <dimension ref="A1:W14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1531,7 +1541,7 @@
         <v>adults</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C5">
         <f>IF(SUMPRODUCT(--(E5:W5&lt;&gt;""))=0,80,"N.A.")</f>
@@ -1793,16 +1803,13 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B14 B2 B11" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"Probability"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>"Duration"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0300-000002000000}">
-      <formula1>"Number"</formula1>
-    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>